<commit_message>
added sprint 1 retrospective, updated sprint 1 burndown, deleted extra folder
</commit_message>
<xml_diff>
--- a/docs/Planning/Sprint1Burndown.xlsx
+++ b/docs/Planning/Sprint1Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/87ed09f771ad8560/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jadeb\Documents\CS 3450\3MusketeersAndARifleman\docs\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="313" documentId="8_{F123FE7E-2449-47A9-9A98-862684C4F296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{388F239C-248D-42F5-B101-F7E083E04D5C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB989B7-7578-4AFA-A243-8B4BF684CFC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5BD6E5F6-9D7D-46B9-9C3C-C2EEC4B0C5B4}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{5BD6E5F6-9D7D-46B9-9C3C-C2EEC4B0C5B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown" sheetId="2" r:id="rId1"/>
@@ -657,7 +657,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1888,7 +1888,7 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1978,7 +1978,9 @@
         <v>10</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="7"/>
+      <c r="I3" s="7">
+        <v>0</v>
+      </c>
       <c r="N3" s="21">
         <v>44609</v>
       </c>
@@ -2010,7 +2012,9 @@
         <v>11</v>
       </c>
       <c r="H4" s="2"/>
-      <c r="I4" s="7"/>
+      <c r="I4" s="7">
+        <v>2</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="N4" s="21">
@@ -2046,7 +2050,9 @@
       <c r="H5" s="2">
         <v>1</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="7">
+        <v>1</v>
+      </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="N5" s="21">
@@ -2085,7 +2091,9 @@
       <c r="H6" s="2">
         <v>2</v>
       </c>
-      <c r="I6" s="7"/>
+      <c r="I6" s="7">
+        <v>0</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="N6" s="21">
@@ -2122,7 +2130,9 @@
         <v>12</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="7"/>
+      <c r="I7" s="7">
+        <v>0</v>
+      </c>
       <c r="K7" s="18"/>
       <c r="L7" s="1"/>
       <c r="N7" s="21">
@@ -2132,7 +2142,7 @@
         <v>0</v>
       </c>
       <c r="P7" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -2255,7 +2265,7 @@
       </c>
       <c r="I12" s="16">
         <f>SUM(I3:I11)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>

</xml_diff>